<commit_message>
Minor fix to inconsistent image and descriptions
</commit_message>
<xml_diff>
--- a/demo-applications/product-retail/datasets/starting-5-product.xlsx
+++ b/demo-applications/product-retail/datasets/starting-5-product.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C0C54E-2B1B-7146-8BBC-87E0B3AEA799}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="30840" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="13" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="491">
   <si>
     <t>Name</t>
   </si>
@@ -564,15 +565,9 @@
     <t>Flat-front dress pant featuring side-slant pockets. The Rossi Straight Fit Slims helps you look smart at work. Whether you are catching a red eye flight or meeting in the boardroom, the Straight Fit Slims adapts to your needs and still allows you to work in style. The Rossi Straight Fit Slims comes with a complementary black leather belt to add an additional accent.</t>
   </si>
   <si>
-    <t>This shirt features a hidden button-down closure with a flap that adds a cleaner, minimalist look. The long sleeves and slim fit style provide a tight fit for the young man on the go. This lightweight shirt is made from high-quality cotton. This shirt is great for a daily look, working for all seasons.</t>
-  </si>
-  <si>
     <t>Blueberry Slim Signature</t>
   </si>
   <si>
-    <t xml:space="preserve">Simple tailored Blueberry Slim Signature blazer is a cropped suit jacket blazer that provides a statement with its signature color ranges. This is a daring blazer designed to draw attention. The long sleeve blazer has a long notched lapel and front dart line to provide a streamlined look and feel. This is the perfect blazer for a casual chic look. The side angled pockets come with a classic aesthetic custom designed to set you apart from anyone else in the room. Enjoy the beautiful and soft velvet texture of the blazer that provides a comfortable and classy look to your outfit. </t>
-  </si>
-  <si>
     <t>Blackberry Slim Pencil Skirt</t>
   </si>
   <si>
@@ -1011,9 +1006,6 @@
     <t>12mm</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1/2 inch</t>
-  </si>
-  <si>
     <t>.5 in</t>
   </si>
   <si>
@@ -1395,9 +1387,6 @@
     <t>https://s3.amazonaws.com/semarchy-tutorials/10057-MAIN.jpg</t>
   </si>
   <si>
-    <t>https://s3.amazonaws.com/semarchy-tutorials/10006-MAIN.jpg</t>
-  </si>
-  <si>
     <t>https://s3.amazonaws.com/semarchy-tutorials/10051-MAIN.jpg</t>
   </si>
   <si>
@@ -1501,6 +1490,9 @@
   </si>
   <si>
     <t>Closure Type</t>
+  </si>
+  <si>
+    <t>EACH</t>
   </si>
 </sst>
 </file>
@@ -4315,28 +4307,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44:H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1"/>
-    <col min="2" max="2" width="64.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="59.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -4347,37 +4339,37 @@
         <v>46</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>487</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>491</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>493</v>
-      </c>
       <c r="M1" s="10" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10075</v>
       </c>
@@ -4397,25 +4389,25 @@
         <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H2" t="s">
         <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>10076</v>
       </c>
@@ -4435,25 +4427,25 @@
         <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H3" t="s">
         <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>10068</v>
       </c>
@@ -4473,25 +4465,25 @@
         <v>66</v>
       </c>
       <c r="G4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H4" t="s">
         <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="L4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>10069</v>
       </c>
@@ -4511,25 +4503,25 @@
         <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="H5" t="s">
         <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>10073</v>
       </c>
@@ -4549,25 +4541,25 @@
         <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H6" t="s">
         <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>10074</v>
       </c>
@@ -4587,25 +4579,25 @@
         <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H7" t="s">
         <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>10070</v>
       </c>
@@ -4625,30 +4617,30 @@
         <v>66</v>
       </c>
       <c r="G8" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="H8" t="s">
         <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>10071</v>
       </c>
       <c r="B9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C9" t="s">
         <v>155</v>
@@ -4663,25 +4655,25 @@
         <v>66</v>
       </c>
       <c r="G9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>10072</v>
       </c>
@@ -4689,7 +4681,7 @@
         <v>106</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
@@ -4701,25 +4693,25 @@
         <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H10" t="s">
         <v>48</v>
       </c>
       <c r="I10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10079</v>
       </c>
@@ -4739,27 +4731,27 @@
         <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="H11" t="s">
         <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J11" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M11" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10081</v>
       </c>
       <c r="B12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C12" t="s">
         <v>164</v>
@@ -4774,27 +4766,27 @@
         <v>66</v>
       </c>
       <c r="G12" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="H12" t="s">
         <v>52</v>
       </c>
       <c r="I12" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M12" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>10080</v>
       </c>
       <c r="B13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C13" t="s">
         <v>163</v>
@@ -4809,22 +4801,22 @@
         <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="H13" t="s">
         <v>52</v>
       </c>
       <c r="I13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J13" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M13" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>10082</v>
       </c>
@@ -4844,22 +4836,22 @@
         <v>66</v>
       </c>
       <c r="G14" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="H14" t="s">
         <v>52</v>
       </c>
       <c r="I14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J14" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M14" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>10065</v>
       </c>
@@ -4879,22 +4871,22 @@
         <v>66</v>
       </c>
       <c r="G15" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="H15" t="s">
         <v>52</v>
       </c>
       <c r="I15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M15" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>10067</v>
       </c>
@@ -4914,22 +4906,22 @@
         <v>66</v>
       </c>
       <c r="G16" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="H16" t="s">
         <v>52</v>
       </c>
       <c r="I16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J16" t="s">
         <v>53</v>
       </c>
       <c r="M16" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>10064</v>
       </c>
@@ -4949,22 +4941,22 @@
         <v>66</v>
       </c>
       <c r="G17" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H17" t="s">
         <v>52</v>
       </c>
       <c r="I17" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J17" t="s">
         <v>49</v>
       </c>
       <c r="M17" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>10066</v>
       </c>
@@ -4984,22 +4976,22 @@
         <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H18" t="s">
         <v>52</v>
       </c>
       <c r="I18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J18" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M18" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>10077</v>
       </c>
@@ -5019,22 +5011,22 @@
         <v>66</v>
       </c>
       <c r="G19" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H19" t="s">
         <v>52</v>
       </c>
       <c r="I19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J19" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M19" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>10078</v>
       </c>
@@ -5054,22 +5046,22 @@
         <v>66</v>
       </c>
       <c r="G20" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H20" t="s">
         <v>52</v>
       </c>
       <c r="I20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J20" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M20" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>10059</v>
       </c>
@@ -5089,22 +5081,22 @@
         <v>66</v>
       </c>
       <c r="G21" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="H21" t="s">
         <v>52</v>
       </c>
       <c r="I21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M21" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>10061</v>
       </c>
@@ -5124,22 +5116,22 @@
         <v>66</v>
       </c>
       <c r="G22" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="H22" t="s">
         <v>52</v>
       </c>
       <c r="I22" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J22" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M22" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>10063</v>
       </c>
@@ -5159,22 +5151,22 @@
         <v>66</v>
       </c>
       <c r="G23" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H23" t="s">
         <v>52</v>
       </c>
       <c r="I23" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J23" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M23" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>10058</v>
       </c>
@@ -5194,22 +5186,22 @@
         <v>66</v>
       </c>
       <c r="G24" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H24" t="s">
         <v>52</v>
       </c>
       <c r="I24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J24" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M24" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>10060</v>
       </c>
@@ -5229,22 +5221,22 @@
         <v>66</v>
       </c>
       <c r="G25" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="H25" t="s">
         <v>52</v>
       </c>
       <c r="I25" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J25" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M25" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>10062</v>
       </c>
@@ -5264,22 +5256,22 @@
         <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="H26" t="s">
         <v>52</v>
       </c>
       <c r="I26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J26" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M26" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>10045</v>
       </c>
@@ -5299,22 +5291,22 @@
         <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="H27" t="s">
         <v>52</v>
       </c>
       <c r="I27" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J27" t="s">
         <v>49</v>
       </c>
       <c r="M27" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>10047</v>
       </c>
@@ -5334,22 +5326,22 @@
         <v>51</v>
       </c>
       <c r="G28" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="H28" t="s">
         <v>52</v>
       </c>
       <c r="I28" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J28" t="s">
         <v>49</v>
       </c>
       <c r="M28" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>10049</v>
       </c>
@@ -5369,22 +5361,22 @@
         <v>51</v>
       </c>
       <c r="G29" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H29" t="s">
         <v>52</v>
       </c>
       <c r="I29" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J29" t="s">
         <v>49</v>
       </c>
       <c r="M29" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>10046</v>
       </c>
@@ -5404,22 +5396,22 @@
         <v>51</v>
       </c>
       <c r="G30" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="H30" t="s">
         <v>52</v>
       </c>
       <c r="I30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J30" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M30" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>10048</v>
       </c>
@@ -5439,22 +5431,22 @@
         <v>51</v>
       </c>
       <c r="G31" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H31" t="s">
         <v>52</v>
       </c>
       <c r="I31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J31" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M31" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>10050</v>
       </c>
@@ -5474,22 +5466,22 @@
         <v>51</v>
       </c>
       <c r="G32" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="H32" t="s">
         <v>52</v>
       </c>
       <c r="I32" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J32" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M32" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>10042</v>
       </c>
@@ -5497,7 +5489,7 @@
         <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -5509,22 +5501,22 @@
         <v>51</v>
       </c>
       <c r="G33" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="H33" t="s">
         <v>52</v>
       </c>
       <c r="I33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="M33" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>10043</v>
       </c>
@@ -5544,22 +5536,22 @@
         <v>51</v>
       </c>
       <c r="G34" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H34" t="s">
         <v>52</v>
       </c>
       <c r="I34" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J34" t="s">
         <v>54</v>
       </c>
       <c r="M34" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>10044</v>
       </c>
@@ -5579,22 +5571,22 @@
         <v>51</v>
       </c>
       <c r="G35" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="H35" t="s">
         <v>52</v>
       </c>
       <c r="I35" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J35" t="s">
         <v>54</v>
       </c>
       <c r="M35" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>10057</v>
       </c>
@@ -5614,22 +5606,22 @@
         <v>51</v>
       </c>
       <c r="G36" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="H36" t="s">
         <v>52</v>
       </c>
       <c r="I36" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J36" t="s">
         <v>49</v>
       </c>
       <c r="M36" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>10051</v>
       </c>
@@ -5649,22 +5641,22 @@
         <v>51</v>
       </c>
       <c r="G37" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="H37" t="s">
         <v>52</v>
       </c>
       <c r="I37" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J37" t="s">
         <v>49</v>
       </c>
       <c r="M37" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>10053</v>
       </c>
@@ -5684,22 +5676,22 @@
         <v>51</v>
       </c>
       <c r="G38" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="H38" t="s">
         <v>52</v>
       </c>
       <c r="I38" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J38" t="s">
         <v>49</v>
       </c>
       <c r="M38" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>10055</v>
       </c>
@@ -5719,22 +5711,22 @@
         <v>51</v>
       </c>
       <c r="G39" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="H39" t="s">
         <v>52</v>
       </c>
       <c r="I39" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J39" t="s">
         <v>49</v>
       </c>
       <c r="M39" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>10052</v>
       </c>
@@ -5754,27 +5746,27 @@
         <v>51</v>
       </c>
       <c r="G40" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="H40" t="s">
         <v>52</v>
       </c>
       <c r="I40" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J40" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M40" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>10054</v>
       </c>
       <c r="B41" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C41" t="s">
         <v>139</v>
@@ -5789,22 +5781,22 @@
         <v>51</v>
       </c>
       <c r="G41" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="H41" t="s">
         <v>52</v>
       </c>
       <c r="I41" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J41" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M41" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>10056</v>
       </c>
@@ -5812,7 +5804,7 @@
         <v>91</v>
       </c>
       <c r="C42" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
@@ -5824,30 +5816,30 @@
         <v>51</v>
       </c>
       <c r="G42" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="H42" t="s">
         <v>52</v>
       </c>
       <c r="I42" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J42" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M42" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>10002</v>
       </c>
       <c r="B43" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C43" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
@@ -5859,22 +5851,22 @@
         <v>75</v>
       </c>
       <c r="G43" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="H43" t="s">
-        <v>52</v>
+        <v>490</v>
       </c>
       <c r="I43" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J43" t="s">
         <v>53</v>
       </c>
       <c r="M43" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>10003</v>
       </c>
@@ -5894,31 +5886,28 @@
         <v>75</v>
       </c>
       <c r="G44" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="H44" t="s">
-        <v>52</v>
+        <v>490</v>
       </c>
       <c r="I44" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J44" t="s">
         <v>49</v>
       </c>
       <c r="M44" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>10004</v>
       </c>
       <c r="B45" t="s">
         <v>69</v>
       </c>
-      <c r="C45" t="s">
-        <v>181</v>
-      </c>
       <c r="D45" t="s">
         <v>7</v>
       </c>
@@ -5929,22 +5918,19 @@
         <v>75</v>
       </c>
       <c r="G45" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H45" t="s">
-        <v>52</v>
-      </c>
-      <c r="I45" t="s">
-        <v>267</v>
+        <v>490</v>
       </c>
       <c r="J45" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M45" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>10001</v>
       </c>
@@ -5964,30 +5950,30 @@
         <v>75</v>
       </c>
       <c r="G46" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H46" t="s">
-        <v>52</v>
+        <v>490</v>
       </c>
       <c r="I46" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J46" t="s">
         <v>49</v>
       </c>
       <c r="M46" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>10005</v>
       </c>
       <c r="B47" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C47" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -5999,22 +5985,22 @@
         <v>75</v>
       </c>
       <c r="G47" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H47" t="s">
-        <v>52</v>
+        <v>490</v>
       </c>
       <c r="I47" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J47" t="s">
         <v>49</v>
       </c>
       <c r="M47" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>10028</v>
       </c>
@@ -6022,7 +6008,7 @@
         <v>74</v>
       </c>
       <c r="C48" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D48" t="s">
         <v>5</v>
@@ -6034,33 +6020,33 @@
         <v>64</v>
       </c>
       <c r="G48" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="H48" t="s">
         <v>48</v>
       </c>
       <c r="I48" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J48" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K48" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L48" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>10029</v>
       </c>
       <c r="B49" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C49" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
@@ -6072,33 +6058,33 @@
         <v>64</v>
       </c>
       <c r="G49" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="H49" t="s">
         <v>48</v>
       </c>
       <c r="I49" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J49" t="s">
         <v>49</v>
       </c>
       <c r="K49" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L49" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>10030</v>
       </c>
       <c r="B50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C50" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D50" t="s">
         <v>5</v>
@@ -6110,33 +6096,33 @@
         <v>64</v>
       </c>
       <c r="G50" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H50" t="s">
         <v>48</v>
       </c>
       <c r="I50" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J50" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K50" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L50" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>10031</v>
       </c>
       <c r="B51" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C51" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D51" t="s">
         <v>5</v>
@@ -6148,33 +6134,33 @@
         <v>64</v>
       </c>
       <c r="G51" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="H51" t="s">
         <v>48</v>
       </c>
       <c r="I51" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J51" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K51" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L51" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>10032</v>
       </c>
       <c r="B52" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C52" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D52" t="s">
         <v>4</v>
@@ -6186,33 +6172,33 @@
         <v>64</v>
       </c>
       <c r="G52" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H52" t="s">
         <v>48</v>
       </c>
       <c r="I52" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J52" t="s">
         <v>49</v>
       </c>
       <c r="K52" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="L52" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>10033</v>
       </c>
       <c r="B53" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C53" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D53" t="s">
         <v>4</v>
@@ -6224,25 +6210,25 @@
         <v>64</v>
       </c>
       <c r="G53" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="H53" t="s">
         <v>48</v>
       </c>
       <c r="I53" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J53" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K53" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L53" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>10013</v>
       </c>
@@ -6250,7 +6236,7 @@
         <v>70</v>
       </c>
       <c r="C54" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D54" t="s">
         <v>9</v>
@@ -6262,30 +6248,30 @@
         <v>60</v>
       </c>
       <c r="G54" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="H54" t="s">
         <v>52</v>
       </c>
       <c r="I54" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J54" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M54" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>10014</v>
       </c>
       <c r="B55" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C55" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
@@ -6297,30 +6283,30 @@
         <v>60</v>
       </c>
       <c r="G55" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="H55" t="s">
         <v>52</v>
       </c>
       <c r="I55" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J55" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M55" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>10015</v>
       </c>
       <c r="B56" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C56" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D56" t="s">
         <v>9</v>
@@ -6332,30 +6318,30 @@
         <v>60</v>
       </c>
       <c r="G56" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H56" t="s">
         <v>52</v>
       </c>
       <c r="I56" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J56" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M56" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>10016</v>
       </c>
       <c r="B57" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C57" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D57" t="s">
         <v>9</v>
@@ -6367,30 +6353,30 @@
         <v>60</v>
       </c>
       <c r="G57" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="H57" t="s">
         <v>52</v>
       </c>
       <c r="I57" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J57" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M57" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>10017</v>
       </c>
       <c r="B58" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C58" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D58" t="s">
         <v>9</v>
@@ -6402,30 +6388,30 @@
         <v>60</v>
       </c>
       <c r="G58" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H58" t="s">
         <v>52</v>
       </c>
       <c r="I58" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J58" t="s">
         <v>49</v>
       </c>
       <c r="M58" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>10010</v>
       </c>
       <c r="B59" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C59" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
@@ -6437,30 +6423,30 @@
         <v>60</v>
       </c>
       <c r="G59" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H59" t="s">
         <v>52</v>
       </c>
       <c r="I59" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J59" t="s">
         <v>49</v>
       </c>
       <c r="M59" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>10022</v>
       </c>
       <c r="B60" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C60" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D60" t="s">
         <v>3</v>
@@ -6472,33 +6458,33 @@
         <v>62</v>
       </c>
       <c r="G60" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="H60" t="s">
         <v>48</v>
       </c>
       <c r="I60" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J60" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K60" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="L60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>10020</v>
       </c>
       <c r="B61" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C61" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D61" t="s">
         <v>3</v>
@@ -6510,33 +6496,33 @@
         <v>62</v>
       </c>
       <c r="G61" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H61" t="s">
         <v>48</v>
       </c>
       <c r="I61" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J61" t="s">
         <v>49</v>
       </c>
       <c r="K61" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L61" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>10021</v>
       </c>
       <c r="B62" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C62" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D62" t="s">
         <v>3</v>
@@ -6548,33 +6534,33 @@
         <v>62</v>
       </c>
       <c r="G62" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H62" t="s">
         <v>48</v>
       </c>
       <c r="I62" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J62" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K62" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L62" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>10038</v>
       </c>
       <c r="B63" t="s">
+        <v>219</v>
+      </c>
+      <c r="C63" t="s">
         <v>221</v>
-      </c>
-      <c r="C63" t="s">
-        <v>223</v>
       </c>
       <c r="D63" t="s">
         <v>2</v>
@@ -6586,33 +6572,33 @@
         <v>65</v>
       </c>
       <c r="G63" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="H63" t="s">
         <v>48</v>
       </c>
       <c r="I63" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J63" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K63" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L63" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>10039</v>
       </c>
       <c r="B64" t="s">
+        <v>220</v>
+      </c>
+      <c r="C64" t="s">
         <v>222</v>
-      </c>
-      <c r="C64" t="s">
-        <v>224</v>
       </c>
       <c r="D64" t="s">
         <v>2</v>
@@ -6624,33 +6610,33 @@
         <v>65</v>
       </c>
       <c r="G64" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="H64" t="s">
         <v>48</v>
       </c>
       <c r="I64" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J64" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K64" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L64" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>10040</v>
       </c>
       <c r="B65" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C65" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D65" t="s">
         <v>2</v>
@@ -6662,33 +6648,33 @@
         <v>65</v>
       </c>
       <c r="G65" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H65" t="s">
         <v>48</v>
       </c>
       <c r="I65" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J65" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K65" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="L65" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>10041</v>
       </c>
       <c r="B66" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C66" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D66" t="s">
         <v>2</v>
@@ -6700,33 +6686,33 @@
         <v>65</v>
       </c>
       <c r="G66" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H66" t="s">
         <v>48</v>
       </c>
       <c r="I66" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J66" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K66" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="L66" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>10034</v>
       </c>
       <c r="B67" t="s">
+        <v>212</v>
+      </c>
+      <c r="C67" t="s">
         <v>214</v>
-      </c>
-      <c r="C67" t="s">
-        <v>216</v>
       </c>
       <c r="D67" t="s">
         <v>3</v>
@@ -6738,33 +6724,33 @@
         <v>65</v>
       </c>
       <c r="G67" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H67" t="s">
         <v>48</v>
       </c>
       <c r="I67" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J67" t="s">
         <v>49</v>
       </c>
       <c r="K67" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="L67" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>10035</v>
       </c>
       <c r="B68" t="s">
+        <v>213</v>
+      </c>
+      <c r="C68" t="s">
         <v>215</v>
-      </c>
-      <c r="C68" t="s">
-        <v>217</v>
       </c>
       <c r="D68" t="s">
         <v>3</v>
@@ -6776,33 +6762,33 @@
         <v>65</v>
       </c>
       <c r="G68" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="H68" t="s">
         <v>48</v>
       </c>
       <c r="I68" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J68" t="s">
         <v>49</v>
       </c>
       <c r="K68" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="L68" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>10036</v>
       </c>
       <c r="B69" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C69" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D69" t="s">
         <v>3</v>
@@ -6814,33 +6800,33 @@
         <v>65</v>
       </c>
       <c r="G69" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H69" t="s">
         <v>48</v>
       </c>
       <c r="I69" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J69" t="s">
         <v>49</v>
       </c>
       <c r="K69" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="L69" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>10037</v>
       </c>
       <c r="B70" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C70" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D70" t="s">
         <v>3</v>
@@ -6852,33 +6838,33 @@
         <v>65</v>
       </c>
       <c r="G70" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="H70" t="s">
         <v>48</v>
       </c>
       <c r="I70" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J70" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K70" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="L70" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>10023</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D71" t="s">
         <v>4</v>
@@ -6890,25 +6876,25 @@
         <v>63</v>
       </c>
       <c r="G71" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="H71" t="s">
         <v>48</v>
       </c>
       <c r="I71" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J71" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K71" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L71" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>10027</v>
       </c>
@@ -6916,7 +6902,7 @@
         <v>73</v>
       </c>
       <c r="C72" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D72" t="s">
         <v>4</v>
@@ -6928,33 +6914,33 @@
         <v>63</v>
       </c>
       <c r="G72" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H72" t="s">
         <v>48</v>
       </c>
       <c r="I72" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="J72" t="s">
         <v>49</v>
       </c>
       <c r="K72" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L72" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>10024</v>
       </c>
       <c r="B73" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C73" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D73" t="s">
         <v>4</v>
@@ -6966,33 +6952,33 @@
         <v>63</v>
       </c>
       <c r="G73" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H73" t="s">
         <v>48</v>
       </c>
       <c r="I73" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J73" t="s">
         <v>49</v>
       </c>
       <c r="K73" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="L73" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>10025</v>
       </c>
       <c r="B74" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C74" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D74" t="s">
         <v>4</v>
@@ -7004,33 +6990,33 @@
         <v>63</v>
       </c>
       <c r="G74" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="H74" t="s">
         <v>48</v>
       </c>
       <c r="I74" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J74" t="s">
         <v>49</v>
       </c>
       <c r="K74" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="L74" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>10026</v>
       </c>
       <c r="B75" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C75" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D75" t="s">
         <v>4</v>
@@ -7042,25 +7028,25 @@
         <v>63</v>
       </c>
       <c r="G75" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="H75" t="s">
         <v>48</v>
       </c>
       <c r="I75" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J75" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K75" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L75" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>10084</v>
       </c>
@@ -7080,30 +7066,30 @@
         <v>77</v>
       </c>
       <c r="G76" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="H76" t="s">
         <v>48</v>
       </c>
       <c r="I76" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J76" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K76" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L76" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>10087</v>
       </c>
       <c r="B77" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C77" t="s">
         <v>170</v>
@@ -7118,25 +7104,25 @@
         <v>77</v>
       </c>
       <c r="G77" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="H77" t="s">
         <v>48</v>
       </c>
       <c r="I77" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J77" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K77" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L77" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>10088</v>
       </c>
@@ -7156,25 +7142,25 @@
         <v>77</v>
       </c>
       <c r="G78" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="H78" t="s">
         <v>48</v>
       </c>
       <c r="I78" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J78" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K78" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L78" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>10091</v>
       </c>
@@ -7194,25 +7180,25 @@
         <v>77</v>
       </c>
       <c r="G79" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="H79" t="s">
         <v>48</v>
       </c>
       <c r="I79" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J79" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K79" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="L79" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>10092</v>
       </c>
@@ -7232,25 +7218,25 @@
         <v>77</v>
       </c>
       <c r="G80" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H80" t="s">
         <v>48</v>
       </c>
       <c r="I80" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J80" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K80" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L80" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>10094</v>
       </c>
@@ -7270,25 +7256,25 @@
         <v>77</v>
       </c>
       <c r="G81" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H81" t="s">
         <v>48</v>
       </c>
       <c r="I81" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J81" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K81" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L81" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>10095</v>
       </c>
@@ -7308,25 +7294,25 @@
         <v>77</v>
       </c>
       <c r="G82" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H82" t="s">
         <v>48</v>
       </c>
       <c r="I82" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J82" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K82" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L82" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>10083</v>
       </c>
@@ -7346,22 +7332,22 @@
         <v>77</v>
       </c>
       <c r="G83" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="H83" t="s">
         <v>52</v>
       </c>
       <c r="I83" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J83" t="s">
         <v>49</v>
       </c>
       <c r="M83" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>10085</v>
       </c>
@@ -7381,22 +7367,22 @@
         <v>77</v>
       </c>
       <c r="G84" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="H84" t="s">
         <v>52</v>
       </c>
       <c r="I84" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J84" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M84" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>10086</v>
       </c>
@@ -7416,22 +7402,22 @@
         <v>77</v>
       </c>
       <c r="G85" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="H85" t="s">
         <v>52</v>
       </c>
       <c r="I85" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J85" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M85" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>10089</v>
       </c>
@@ -7451,22 +7437,22 @@
         <v>77</v>
       </c>
       <c r="G86" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="H86" t="s">
         <v>52</v>
       </c>
       <c r="I86" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J86" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M86" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>10090</v>
       </c>
@@ -7486,22 +7472,22 @@
         <v>77</v>
       </c>
       <c r="G87" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H87" t="s">
         <v>52</v>
       </c>
       <c r="I87" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J87" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M87" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>10093</v>
       </c>
@@ -7521,22 +7507,22 @@
         <v>77</v>
       </c>
       <c r="G88" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="H88" t="s">
         <v>52</v>
       </c>
       <c r="I88" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J88" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M88" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>10096</v>
       </c>
@@ -7544,7 +7530,7 @@
         <v>127</v>
       </c>
       <c r="C89" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D89" t="s">
         <v>6</v>
@@ -7556,22 +7542,22 @@
         <v>77</v>
       </c>
       <c r="G89" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="H89" t="s">
         <v>52</v>
       </c>
       <c r="I89" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J89" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M89" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>10018</v>
       </c>
@@ -7579,7 +7565,7 @@
         <v>71</v>
       </c>
       <c r="C90" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D90" t="s">
         <v>2</v>
@@ -7591,25 +7577,25 @@
         <v>61</v>
       </c>
       <c r="G90" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="H90" t="s">
         <v>48</v>
       </c>
       <c r="I90" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J90" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K90" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L90" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>10019</v>
       </c>
@@ -7617,7 +7603,7 @@
         <v>72</v>
       </c>
       <c r="C91" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D91" t="s">
         <v>2</v>
@@ -7629,33 +7615,30 @@
         <v>61</v>
       </c>
       <c r="G91" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="H91" t="s">
         <v>48</v>
       </c>
       <c r="I91" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J91" t="s">
+        <v>314</v>
+      </c>
+      <c r="K91" t="s">
         <v>316</v>
-      </c>
-      <c r="K91" t="s">
-        <v>318</v>
       </c>
       <c r="L91" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>10006</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
-      </c>
-      <c r="C92" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
@@ -7666,31 +7649,25 @@
       <c r="F92" t="s">
         <v>76</v>
       </c>
-      <c r="G92" t="s">
-        <v>458</v>
-      </c>
       <c r="H92" t="s">
         <v>52</v>
       </c>
       <c r="I92" t="s">
-        <v>271</v>
-      </c>
-      <c r="J92" t="s">
-        <v>49</v>
+        <v>269</v>
       </c>
       <c r="M92" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>10007</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C93" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
@@ -7702,30 +7679,30 @@
         <v>76</v>
       </c>
       <c r="G93" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="H93" t="s">
         <v>52</v>
       </c>
       <c r="I93" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J93" t="s">
         <v>49</v>
       </c>
       <c r="M93" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>10008</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C94" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -7737,30 +7714,30 @@
         <v>76</v>
       </c>
       <c r="G94" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="H94" t="s">
         <v>52</v>
       </c>
       <c r="I94" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J94" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M94" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>10009</v>
       </c>
       <c r="B95" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C95" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
@@ -7772,27 +7749,27 @@
         <v>76</v>
       </c>
       <c r="G95" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="H95" t="s">
         <v>52</v>
       </c>
       <c r="I95" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J95" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M95" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>10100</v>
       </c>
       <c r="B96" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C96" t="s">
         <v>158</v>
@@ -7807,30 +7784,30 @@
         <v>66</v>
       </c>
       <c r="G96" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="H96" t="s">
         <v>48</v>
       </c>
       <c r="I96" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J96" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K96" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L96" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>10101</v>
       </c>
       <c r="B97" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C97" t="s">
         <v>159</v>
@@ -7845,33 +7822,33 @@
         <v>66</v>
       </c>
       <c r="G97" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H97" t="s">
         <v>48</v>
       </c>
       <c r="I97" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J97" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K97" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L97" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>10102</v>
       </c>
       <c r="B98" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C98" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D98" t="s">
         <v>3</v>
@@ -7880,33 +7857,33 @@
         <v>13</v>
       </c>
       <c r="G98" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H98" t="s">
         <v>48</v>
       </c>
       <c r="I98" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J98" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K98" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L98" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>10103</v>
       </c>
       <c r="B99" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D99" t="s">
         <v>3</v>
@@ -7915,51 +7892,51 @@
         <v>13</v>
       </c>
       <c r="G99" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H99" t="s">
         <v>48</v>
       </c>
       <c r="I99" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J99" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="K99" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L99" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>10104</v>
       </c>
       <c r="B100" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C100" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="E100" t="s">
         <v>43</v>
       </c>
       <c r="G100" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="H100" t="s">
         <v>52</v>
       </c>
       <c r="I100" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J100" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M100" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Product Retail tutorial for v5.2 incl. new features & screenshots
</commit_message>
<xml_diff>
--- a/demo-applications/product-retail/datasets/starting-5-product.xlsx
+++ b/demo-applications/product-retail/datasets/starting-5-product.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C0C54E-2B1B-7146-8BBC-87E0B3AEA799}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94B57AD-53C4-2D43-B348-7EEBD806642D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="30840" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34620" yWindow="3180" windowWidth="30840" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="13" r:id="rId1"/>
@@ -1441,9 +1441,6 @@
     <t>Wonder World Cupcake Sprinkle High tops</t>
   </si>
   <si>
-    <t>Aquaplenish Water Aerobics Trainers</t>
-  </si>
-  <si>
     <t>Flexible water aerobics shoe designed for water aerobic classes. Anti-slip and comfortable in the water.</t>
   </si>
   <si>
@@ -1493,6 +1490,9 @@
   </si>
   <si>
     <t>EACH</t>
+  </si>
+  <si>
+    <t>Milliped Water Aerobics Trainers</t>
   </si>
 </sst>
 </file>
@@ -4307,8 +4307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44:H47"/>
+    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4339,34 +4339,34 @@
         <v>46</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>482</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>484</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J1" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="10" t="s">
         <v>485</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>489</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -4918,7 +4918,7 @@
         <v>53</v>
       </c>
       <c r="M16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -5854,7 +5854,7 @@
         <v>436</v>
       </c>
       <c r="H43" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I43" t="s">
         <v>256</v>
@@ -5889,7 +5889,7 @@
         <v>440</v>
       </c>
       <c r="H44" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I44" t="s">
         <v>257</v>
@@ -5921,7 +5921,7 @@
         <v>445</v>
       </c>
       <c r="H45" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J45" t="s">
         <v>312</v>
@@ -5953,7 +5953,7 @@
         <v>452</v>
       </c>
       <c r="H46" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I46" t="s">
         <v>255</v>
@@ -5988,7 +5988,7 @@
         <v>453</v>
       </c>
       <c r="H47" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I47" t="s">
         <v>286</v>
@@ -7807,7 +7807,7 @@
         <v>10101</v>
       </c>
       <c r="B97" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C97" t="s">
         <v>159</v>
@@ -7845,10 +7845,10 @@
         <v>10102</v>
       </c>
       <c r="B98" t="s">
+        <v>490</v>
+      </c>
+      <c r="C98" t="s">
         <v>473</v>
-      </c>
-      <c r="C98" t="s">
-        <v>474</v>
       </c>
       <c r="D98" t="s">
         <v>3</v>
@@ -7880,10 +7880,10 @@
         <v>10103</v>
       </c>
       <c r="B99" t="s">
+        <v>474</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>475</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>476</v>
       </c>
       <c r="D99" t="s">
         <v>3</v>
@@ -7915,10 +7915,10 @@
         <v>10104</v>
       </c>
       <c r="B100" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C100" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E100" t="s">
         <v>43</v>
@@ -7940,7 +7940,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:M95">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M95">
     <sortCondition ref="F2:F95"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>